<commit_message>
fixed mag naming mistakes
</commit_message>
<xml_diff>
--- a/figures_and_tables/Table_S1.xlsx
+++ b/figures_and_tables/Table_S1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="8780" windowWidth="42220" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="22080" yWindow="2020" windowWidth="24520" windowHeight="24340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="210">
   <si>
     <t>N50</t>
   </si>
@@ -305,9 +305,6 @@
     <t>bin.9</t>
   </si>
   <si>
-    <t>bin.algae</t>
-  </si>
-  <si>
     <t>Archaea;Euryarchaeota;Halobacteria</t>
   </si>
   <si>
@@ -320,9 +317,6 @@
     <t>Archaea;Euryarchaeota;Halobacteria;Haloferacales;Haloferacaceae</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Archaea;Candidatus Nanohaloarchaeota;Nanohaloarchaea</t>
   </si>
   <si>
@@ -347,12 +341,6 @@
     <t>Bacteria;Proteobacteria;Deltaproteobacteria</t>
   </si>
   <si>
-    <t>Eukaria;Plantae;Chlorophyta</t>
-  </si>
-  <si>
-    <t>bin.chloroplast</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bacteria;Terrabacteria group;Cyanobacteria;Cyanobacteria;Oscillatoriophycideae;Chroococcales;Aphanothecaceae;Halothece cluster;Halothece </t>
   </si>
   <si>
@@ -656,24 +644,35 @@
     <t>SG1_Halothece_65_4</t>
   </si>
   <si>
-    <t>SG1_Chlorophyta_56_24</t>
-  </si>
-  <si>
     <t>MAG name</t>
   </si>
   <si>
     <t>bin name</t>
   </si>
   <si>
-    <t>SG1_ChlorophytaChpl_40_179</t>
+    <t>SG1_Halobacteriaceae_70_6</t>
+  </si>
+  <si>
+    <t>SG1_Halobacteriaceae_67_9</t>
+  </si>
+  <si>
+    <t>SG1_Halobacteriaceae_65_25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -701,8 +700,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K94"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,384 +998,384 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" t="s">
         <v>115</v>
       </c>
-      <c r="I1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" t="s">
-        <v>119</v>
-      </c>
       <c r="K1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C2">
-        <v>84.03</v>
+        <v>81.540000000000006</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="E2">
-        <v>0.44900000000000001</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="F2">
-        <v>13350</v>
+        <v>4218</v>
       </c>
       <c r="G2">
-        <v>887108</v>
+        <v>2612197</v>
       </c>
       <c r="H2">
-        <v>85</v>
+        <v>725</v>
       </c>
       <c r="I2">
-        <v>7.7114099999999999</v>
+        <v>5.6522800000000002</v>
       </c>
       <c r="J2">
-        <v>0.175100948422</v>
+        <v>1.47342059872</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C3">
-        <v>89.4</v>
+        <v>85.75</v>
       </c>
       <c r="D3">
-        <v>1.869</v>
+        <v>0.8</v>
       </c>
       <c r="E3">
-        <v>0.44700000000000001</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="F3">
-        <v>268131</v>
+        <v>4801</v>
       </c>
       <c r="G3">
-        <v>1037184</v>
+        <v>2415797</v>
       </c>
       <c r="H3">
-        <v>17</v>
+        <v>633</v>
       </c>
       <c r="I3">
-        <v>9.8953600000000002</v>
+        <v>7.2144700000000004</v>
       </c>
       <c r="J3">
-        <v>0.108350626666</v>
+        <v>13.5394742311</v>
       </c>
       <c r="K3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C4">
-        <v>87.14</v>
+        <v>93.84</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2.1360000000000001</v>
       </c>
       <c r="E4">
-        <v>0.46400000000000002</v>
+        <v>0.73</v>
       </c>
       <c r="F4">
-        <v>43621</v>
+        <v>11979</v>
       </c>
       <c r="G4">
-        <v>1097787</v>
+        <v>2413993</v>
       </c>
       <c r="H4">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="I4">
-        <v>23.054200000000002</v>
+        <v>18.581099999999999</v>
       </c>
       <c r="J4">
-        <v>0.15690615322699999</v>
+        <v>3.7820669748000002</v>
       </c>
       <c r="K4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <v>92.77</v>
+        <v>91.25</v>
       </c>
       <c r="D5">
-        <v>1.2609999999999999</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.64</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="F5">
-        <v>8885</v>
+        <v>8200</v>
       </c>
       <c r="G5">
-        <v>2809869</v>
+        <v>2655338</v>
       </c>
       <c r="H5">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="I5">
-        <v>42.1295</v>
+        <v>5.77658</v>
       </c>
       <c r="J5">
-        <v>0.917173481023</v>
+        <v>0.93849831142700002</v>
       </c>
       <c r="K5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C6">
-        <v>79.5</v>
+        <v>81.03</v>
       </c>
       <c r="D6">
-        <v>1.306</v>
+        <v>1.724</v>
       </c>
       <c r="E6">
-        <v>0.64700000000000002</v>
+        <v>0.502</v>
       </c>
       <c r="F6">
-        <v>5805</v>
+        <v>4473</v>
       </c>
       <c r="G6">
-        <v>2613039</v>
+        <v>785653</v>
       </c>
       <c r="H6">
-        <v>573</v>
+        <v>226</v>
       </c>
       <c r="I6">
-        <v>46.765000000000001</v>
+        <v>6.4623999999999997</v>
       </c>
       <c r="J6">
-        <v>8.9017159863999995E-2</v>
+        <v>1.04182866076</v>
       </c>
       <c r="K6" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>85.94</v>
+        <v>80.08</v>
       </c>
       <c r="D7">
-        <v>0.89500000000000002</v>
+        <v>2.23</v>
       </c>
       <c r="E7">
-        <v>0.69699999999999995</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="F7">
-        <v>4624</v>
+        <v>3687</v>
       </c>
       <c r="G7">
-        <v>2951147</v>
+        <v>2200091</v>
       </c>
       <c r="H7">
-        <v>685</v>
+        <v>568</v>
       </c>
       <c r="I7">
-        <v>16.8964</v>
+        <v>22.8489</v>
       </c>
       <c r="J7">
-        <v>2.0024628492200001</v>
+        <v>0.94885614727099998</v>
       </c>
       <c r="K7" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C8">
-        <v>92.51</v>
+        <v>78.83</v>
       </c>
       <c r="D8">
-        <v>2.6150000000000002</v>
+        <v>2.41</v>
       </c>
       <c r="E8">
-        <v>0.57299999999999995</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="F8">
-        <v>6484</v>
+        <v>4365</v>
       </c>
       <c r="G8">
-        <v>2678007</v>
+        <v>4202192</v>
       </c>
       <c r="H8">
-        <v>469</v>
+        <v>1030</v>
       </c>
       <c r="I8">
-        <v>7.0010500000000002</v>
+        <v>4.6524599999999996</v>
       </c>
       <c r="J8">
-        <v>0.58163408726599997</v>
+        <v>0.10902753425099999</v>
       </c>
       <c r="K8" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>74.77</v>
+        <v>95.48</v>
       </c>
       <c r="D9">
-        <v>2.2000000000000002</v>
+        <v>1.2070000000000001</v>
       </c>
       <c r="E9">
-        <v>0.68799999999999994</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="F9">
-        <v>4199</v>
+        <v>8367</v>
       </c>
       <c r="G9">
-        <v>1595022</v>
+        <v>2396020</v>
       </c>
       <c r="H9">
-        <v>476</v>
+        <v>333</v>
       </c>
       <c r="I9">
-        <v>28.463100000000001</v>
+        <v>7.76295</v>
       </c>
       <c r="J9">
-        <v>0.49732626714099998</v>
+        <v>18.302453766599999</v>
       </c>
       <c r="K9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>202</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C10">
-        <v>89.27</v>
+        <v>97.77</v>
       </c>
       <c r="D10">
-        <v>1.7949999999999999</v>
+        <v>0.222</v>
       </c>
       <c r="E10">
-        <v>0.65</v>
+        <v>0.439</v>
       </c>
       <c r="F10">
-        <v>8023</v>
+        <v>18977</v>
       </c>
       <c r="G10">
-        <v>3353205</v>
+        <v>3489855</v>
       </c>
       <c r="H10">
-        <v>536</v>
+        <v>345</v>
       </c>
       <c r="I10">
-        <v>130.911</v>
+        <v>8.2834400000000006</v>
       </c>
       <c r="J10">
-        <v>0.13579278440199999</v>
+        <v>595.33637534000002</v>
       </c>
       <c r="K10" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C11">
-        <v>80.88</v>
+        <v>80.97</v>
       </c>
       <c r="D11">
-        <v>3.5659999999999998</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.69599999999999995</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="F11">
-        <v>3806</v>
+        <v>5268</v>
       </c>
       <c r="G11">
-        <v>2876592</v>
+        <v>616685</v>
       </c>
       <c r="H11">
-        <v>779</v>
+        <v>132</v>
       </c>
       <c r="I11">
-        <v>12.9329</v>
+        <v>7.5327400000000004</v>
       </c>
       <c r="J11">
-        <v>1.0886963119599999</v>
+        <v>4.4299352804899996</v>
       </c>
       <c r="K11" t="s">
         <v>93</v>
@@ -1383,392 +1383,392 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>84.9</v>
+        <v>92.51</v>
       </c>
       <c r="D12">
-        <v>2.3610000000000002</v>
+        <v>2.6150000000000002</v>
       </c>
       <c r="E12">
-        <v>0.67800000000000005</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="F12">
-        <v>4503</v>
+        <v>6484</v>
       </c>
       <c r="G12">
-        <v>2488760</v>
+        <v>2678007</v>
       </c>
       <c r="H12">
-        <v>624</v>
+        <v>469</v>
       </c>
       <c r="I12">
-        <v>16.407499999999999</v>
+        <v>7.0010500000000002</v>
       </c>
       <c r="J12">
-        <v>2.4307553027400002</v>
+        <v>0.58163408726599997</v>
       </c>
       <c r="K12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13">
-        <v>79.2</v>
+        <v>71.72</v>
       </c>
       <c r="D13">
-        <v>1.333</v>
+        <v>4.7149999999999999</v>
       </c>
       <c r="E13">
-        <v>0.64300000000000002</v>
+        <v>0.625</v>
       </c>
       <c r="F13">
-        <v>4142</v>
+        <v>2678</v>
       </c>
       <c r="G13">
-        <v>2119876</v>
+        <v>1945603</v>
       </c>
       <c r="H13">
-        <v>538</v>
+        <v>777</v>
       </c>
       <c r="I13">
-        <v>5.5636000000000001</v>
+        <v>5.8210600000000001</v>
       </c>
       <c r="J13">
-        <v>1.4116477301200001</v>
+        <v>1.3068086532300001</v>
       </c>
       <c r="K13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>71.72</v>
+        <v>92.77</v>
       </c>
       <c r="D14">
-        <v>4.7149999999999999</v>
+        <v>1.2609999999999999</v>
       </c>
       <c r="E14">
-        <v>0.625</v>
+        <v>0.64</v>
       </c>
       <c r="F14">
-        <v>2678</v>
+        <v>8885</v>
       </c>
       <c r="G14">
-        <v>1945603</v>
+        <v>2809869</v>
       </c>
       <c r="H14">
-        <v>777</v>
+        <v>415</v>
       </c>
       <c r="I14">
-        <v>5.8210600000000001</v>
+        <v>42.1295</v>
       </c>
       <c r="J14">
-        <v>1.3068086532300001</v>
+        <v>0.917173481023</v>
       </c>
       <c r="K14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C15">
-        <v>95.95</v>
+        <v>79.2</v>
       </c>
       <c r="D15">
-        <v>1.7250000000000001</v>
+        <v>1.333</v>
       </c>
       <c r="E15">
-        <v>0.67600000000000005</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="F15">
-        <v>18319</v>
+        <v>4142</v>
       </c>
       <c r="G15">
-        <v>2506034</v>
+        <v>2119876</v>
       </c>
       <c r="H15">
-        <v>181</v>
+        <v>538</v>
       </c>
       <c r="I15">
-        <v>17.506499999999999</v>
+        <v>5.5636000000000001</v>
       </c>
       <c r="J15">
-        <v>22.502860401300001</v>
+        <v>1.4116477301200001</v>
       </c>
       <c r="K15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C16">
-        <v>82.99</v>
+        <v>89.27</v>
       </c>
       <c r="D16">
-        <v>1.766</v>
+        <v>1.7949999999999999</v>
       </c>
       <c r="E16">
         <v>0.65</v>
       </c>
       <c r="F16">
-        <v>6238</v>
+        <v>8023</v>
       </c>
       <c r="G16">
-        <v>2722551</v>
+        <v>3353205</v>
       </c>
       <c r="H16">
-        <v>515</v>
+        <v>536</v>
       </c>
       <c r="I16">
-        <v>8.92727</v>
+        <v>130.911</v>
       </c>
       <c r="J16">
-        <v>0.54075306066999995</v>
+        <v>0.13579278440199999</v>
       </c>
       <c r="K16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>90.71</v>
+        <v>79.5</v>
       </c>
       <c r="D17">
-        <v>1.0629999999999999</v>
+        <v>1.306</v>
       </c>
       <c r="E17">
-        <v>0.66400000000000003</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="F17">
-        <v>7300</v>
+        <v>5805</v>
       </c>
       <c r="G17">
-        <v>3089989</v>
+        <v>2613039</v>
       </c>
       <c r="H17">
-        <v>522</v>
+        <v>573</v>
       </c>
       <c r="I17">
-        <v>12.8184</v>
+        <v>46.765000000000001</v>
       </c>
       <c r="J17">
-        <v>2.0940784289600001</v>
+        <v>8.9017159863999995E-2</v>
       </c>
       <c r="K17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C18">
-        <v>78.010000000000005</v>
+        <v>82.99</v>
       </c>
       <c r="D18">
-        <v>1.0660000000000001</v>
+        <v>1.766</v>
       </c>
       <c r="E18">
-        <v>0.67700000000000005</v>
+        <v>0.65</v>
       </c>
       <c r="F18">
-        <v>3525</v>
+        <v>6238</v>
       </c>
       <c r="G18">
-        <v>1618410</v>
+        <v>2722551</v>
       </c>
       <c r="H18">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="I18">
-        <v>34.844299999999997</v>
+        <v>8.92727</v>
       </c>
       <c r="J18">
-        <v>0.26388768918</v>
+        <v>0.54075306066999995</v>
       </c>
       <c r="K18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>70.94</v>
+        <v>90.71</v>
       </c>
       <c r="D19">
-        <v>3.24</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="E19">
-        <v>0.67</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="F19">
-        <v>4890</v>
+        <v>7300</v>
       </c>
       <c r="G19">
-        <v>2329581</v>
+        <v>3089989</v>
       </c>
       <c r="H19">
-        <v>538</v>
+        <v>522</v>
       </c>
       <c r="I19">
-        <v>10.7239</v>
+        <v>12.8184</v>
       </c>
       <c r="J19">
-        <v>1.39840536843</v>
+        <v>2.0940784289600001</v>
       </c>
       <c r="K19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C20">
-        <v>89.92</v>
+        <v>90.86</v>
       </c>
       <c r="D20">
-        <v>2.0659999999999998</v>
+        <v>1.718</v>
       </c>
       <c r="E20">
         <v>0.65700000000000003</v>
       </c>
       <c r="F20">
-        <v>6380</v>
+        <v>14371</v>
       </c>
       <c r="G20">
-        <v>2466435</v>
+        <v>2956102</v>
       </c>
       <c r="H20">
-        <v>483</v>
+        <v>282</v>
       </c>
       <c r="I20">
-        <v>14.5253</v>
+        <v>14.3134</v>
       </c>
       <c r="J20">
-        <v>12.809189917399999</v>
+        <v>8.2040361971499998</v>
       </c>
       <c r="K20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C21">
-        <v>89.18</v>
+        <v>89.92</v>
       </c>
       <c r="D21">
-        <v>1.448</v>
+        <v>2.0659999999999998</v>
       </c>
       <c r="E21">
-        <v>0.73</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="F21">
-        <v>10870</v>
+        <v>6380</v>
       </c>
       <c r="G21">
-        <v>2670516</v>
+        <v>2466435</v>
       </c>
       <c r="H21">
-        <v>259</v>
+        <v>483</v>
       </c>
       <c r="I21">
-        <v>11.014099999999999</v>
+        <v>14.5253</v>
       </c>
       <c r="J21">
-        <v>9.4233639013099992</v>
+        <v>12.809189917399999</v>
       </c>
       <c r="K21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C22">
-        <v>90.86</v>
+        <v>70.94</v>
       </c>
       <c r="D22">
-        <v>1.718</v>
+        <v>3.24</v>
       </c>
       <c r="E22">
-        <v>0.65700000000000003</v>
+        <v>0.67</v>
       </c>
       <c r="F22">
-        <v>14371</v>
+        <v>4890</v>
       </c>
       <c r="G22">
-        <v>2956102</v>
+        <v>2329581</v>
       </c>
       <c r="H22">
-        <v>282</v>
+        <v>538</v>
       </c>
       <c r="I22">
-        <v>14.3134</v>
+        <v>10.7239</v>
       </c>
       <c r="J22">
-        <v>8.2040361971499998</v>
+        <v>1.39840536843</v>
       </c>
       <c r="K22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B23" t="s">
         <v>82</v>
@@ -1798,672 +1798,672 @@
         <v>0.88631236760300003</v>
       </c>
       <c r="K23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="C24">
-        <v>74.150000000000006</v>
+        <v>84.9</v>
       </c>
       <c r="D24">
-        <v>4.9640000000000004</v>
+        <v>2.3610000000000002</v>
       </c>
       <c r="E24">
-        <v>0.70399999999999996</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="F24">
-        <v>4509</v>
+        <v>4503</v>
       </c>
       <c r="G24">
-        <v>2540070</v>
+        <v>2488760</v>
       </c>
       <c r="H24">
-        <v>696</v>
+        <v>624</v>
       </c>
       <c r="I24">
-        <v>19.0215</v>
+        <v>16.407499999999999</v>
       </c>
       <c r="J24">
-        <v>0.69308638187100002</v>
+        <v>2.4307553027400002</v>
       </c>
       <c r="K24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C25">
-        <v>72.180000000000007</v>
+        <v>95.95</v>
       </c>
       <c r="D25">
-        <v>1.0629999999999999</v>
+        <v>1.7250000000000001</v>
       </c>
       <c r="E25">
-        <v>0.66800000000000004</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="F25">
-        <v>8025</v>
+        <v>18319</v>
       </c>
       <c r="G25">
-        <v>1841689</v>
+        <v>2506034</v>
       </c>
       <c r="H25">
-        <v>310</v>
+        <v>181</v>
       </c>
       <c r="I25">
-        <v>5.4245700000000001</v>
+        <v>17.506499999999999</v>
       </c>
       <c r="J25">
-        <v>1.82360146632</v>
+        <v>22.502860401300001</v>
       </c>
       <c r="K25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C26">
-        <v>75.150000000000006</v>
+        <v>78.010000000000005</v>
       </c>
       <c r="D26">
-        <v>2.2149999999999999</v>
+        <v>1.0660000000000001</v>
       </c>
       <c r="E26">
-        <v>0.68799999999999994</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="F26">
-        <v>2789</v>
+        <v>3525</v>
       </c>
       <c r="G26">
-        <v>2616278</v>
+        <v>1618410</v>
       </c>
       <c r="H26">
-        <v>1008</v>
+        <v>519</v>
       </c>
       <c r="I26">
-        <v>49.792499999999997</v>
+        <v>34.844299999999997</v>
       </c>
       <c r="J26">
-        <v>0.52071066669099997</v>
+        <v>0.26388768918</v>
       </c>
       <c r="K26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>86.96</v>
+        <v>74.77</v>
       </c>
       <c r="D27">
-        <v>1.276</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E27">
-        <v>0.70599999999999996</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="F27">
-        <v>4885</v>
+        <v>4199</v>
       </c>
       <c r="G27">
-        <v>2115032</v>
+        <v>1595022</v>
       </c>
       <c r="H27">
-        <v>508</v>
+        <v>476</v>
       </c>
       <c r="I27">
-        <v>21.4267</v>
+        <v>28.463100000000001</v>
       </c>
       <c r="J27">
-        <v>0.85589581425299999</v>
+        <v>0.49732626714099998</v>
       </c>
       <c r="K27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C28">
-        <v>87.75</v>
+        <v>80.88</v>
       </c>
       <c r="D28">
-        <v>1.762</v>
+        <v>3.5659999999999998</v>
       </c>
       <c r="E28">
         <v>0.69599999999999995</v>
       </c>
       <c r="F28">
-        <v>4711</v>
+        <v>3806</v>
       </c>
       <c r="G28">
-        <v>2778251</v>
+        <v>2876592</v>
       </c>
       <c r="H28">
-        <v>636</v>
+        <v>779</v>
       </c>
       <c r="I28">
-        <v>58.559199999999997</v>
+        <v>12.9329</v>
       </c>
       <c r="J28">
-        <v>0.66381948452299999</v>
+        <v>1.0886963119599999</v>
       </c>
       <c r="K28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>89.63</v>
+        <v>85.94</v>
       </c>
       <c r="D29">
-        <v>2.3559999999999999</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="E29">
-        <v>0.68700000000000006</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="F29">
-        <v>12405</v>
+        <v>4624</v>
       </c>
       <c r="G29">
-        <v>2703765</v>
+        <v>2951147</v>
       </c>
       <c r="H29">
-        <v>277</v>
+        <v>685</v>
       </c>
       <c r="I29">
-        <v>8.4095300000000002</v>
+        <v>16.8964</v>
       </c>
       <c r="J29">
-        <v>1.6983139973200001</v>
+        <v>2.0024628492200001</v>
       </c>
       <c r="K29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="C30">
-        <v>82.72</v>
+        <v>74.150000000000006</v>
       </c>
       <c r="D30">
-        <v>4.415</v>
+        <v>4.9640000000000004</v>
       </c>
       <c r="E30">
-        <v>0.7</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="F30">
-        <v>6886</v>
+        <v>4509</v>
       </c>
       <c r="G30">
-        <v>2162581</v>
+        <v>2540070</v>
       </c>
       <c r="H30">
-        <v>391</v>
+        <v>696</v>
       </c>
       <c r="I30">
-        <v>7.6546000000000003</v>
+        <v>19.0215</v>
       </c>
       <c r="J30">
-        <v>8.4782114963099993</v>
+        <v>0.69308638187100002</v>
       </c>
       <c r="K30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="C31">
-        <v>81.23</v>
+        <v>89.18</v>
       </c>
       <c r="D31">
-        <v>2.1659999999999999</v>
+        <v>1.448</v>
       </c>
       <c r="E31">
-        <v>0.63700000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="F31">
-        <v>5164</v>
+        <v>10870</v>
       </c>
       <c r="G31">
-        <v>2793438</v>
+        <v>2670516</v>
       </c>
       <c r="H31">
-        <v>692</v>
+        <v>259</v>
       </c>
       <c r="I31">
-        <v>14.3535</v>
+        <v>11.014099999999999</v>
       </c>
       <c r="J31">
-        <v>8.5043864516899994</v>
+        <v>9.4233639013099992</v>
       </c>
       <c r="K31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C32">
-        <v>72.989999999999995</v>
+        <v>89.84</v>
       </c>
       <c r="D32">
-        <v>1.2330000000000001</v>
+        <v>1.47</v>
       </c>
       <c r="E32">
-        <v>0.66300000000000003</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="F32">
-        <v>5746</v>
+        <v>4846</v>
       </c>
       <c r="G32">
-        <v>1892619</v>
+        <v>1906484</v>
       </c>
       <c r="H32">
-        <v>390</v>
+        <v>449</v>
       </c>
       <c r="I32">
-        <v>7.2593699999999997</v>
+        <v>4.26478</v>
       </c>
       <c r="J32">
-        <v>8.2451564577200003</v>
+        <v>27.5250529333</v>
       </c>
       <c r="K32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="C33">
-        <v>81.7</v>
+        <v>81.040000000000006</v>
       </c>
       <c r="D33">
-        <v>1.6659999999999999</v>
+        <v>3.133</v>
       </c>
       <c r="E33">
-        <v>0.70299999999999996</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="F33">
-        <v>4157</v>
+        <v>5061</v>
       </c>
       <c r="G33">
-        <v>2602580</v>
+        <v>2694110</v>
       </c>
       <c r="H33">
-        <v>689</v>
+        <v>614</v>
       </c>
       <c r="I33">
-        <v>7.2685000000000004</v>
+        <v>4.9092599999999997</v>
       </c>
       <c r="J33">
-        <v>3.9312230735</v>
+        <v>1.5635214425899999</v>
       </c>
       <c r="K33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="C34">
-        <v>82.9</v>
+        <v>93.99</v>
       </c>
       <c r="D34">
-        <v>3.2970000000000002</v>
+        <v>1.3149999999999999</v>
       </c>
       <c r="E34">
-        <v>0.69</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="F34">
-        <v>4364</v>
+        <v>9051</v>
       </c>
       <c r="G34">
-        <v>3093298</v>
+        <v>2064438</v>
       </c>
       <c r="H34">
-        <v>922</v>
+        <v>283</v>
       </c>
       <c r="I34">
-        <v>119.285</v>
+        <v>7.6235299999999997</v>
       </c>
       <c r="J34">
-        <v>3.13323336337</v>
+        <v>0.17205142108599999</v>
       </c>
       <c r="K34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C35">
-        <v>72.47</v>
+        <v>81.23</v>
       </c>
       <c r="D35">
-        <v>1.8</v>
+        <v>2.1659999999999999</v>
       </c>
       <c r="E35">
-        <v>0.65700000000000003</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="F35">
-        <v>3389</v>
+        <v>5164</v>
       </c>
       <c r="G35">
-        <v>2173558</v>
+        <v>2793438</v>
       </c>
       <c r="H35">
-        <v>739</v>
+        <v>692</v>
       </c>
       <c r="I35">
-        <v>56.4711</v>
+        <v>14.3535</v>
       </c>
       <c r="J35">
-        <v>3.2386193518900002</v>
+        <v>8.5043864516899994</v>
       </c>
       <c r="K35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C36">
-        <v>81.87</v>
+        <v>79.23</v>
       </c>
       <c r="D36">
-        <v>5.46</v>
+        <v>1.702</v>
       </c>
       <c r="E36">
-        <v>0.67700000000000005</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="F36">
-        <v>4231</v>
+        <v>5323</v>
       </c>
       <c r="G36">
-        <v>2422757</v>
+        <v>2236126</v>
       </c>
       <c r="H36">
-        <v>626</v>
+        <v>498</v>
       </c>
       <c r="I36">
-        <v>34.419699999999999</v>
+        <v>4.9612499999999997</v>
       </c>
       <c r="J36">
-        <v>23.307644699899999</v>
+        <v>22.363607848699999</v>
       </c>
       <c r="K36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C37">
-        <v>94.84</v>
+        <v>97.05</v>
       </c>
       <c r="D37">
-        <v>2.8149999999999999</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="E37">
-        <v>0.66600000000000004</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="F37">
-        <v>12192</v>
+        <v>36692</v>
       </c>
       <c r="G37">
-        <v>3181126</v>
+        <v>1787608</v>
       </c>
       <c r="H37">
-        <v>354</v>
+        <v>56</v>
       </c>
       <c r="I37">
-        <v>9.5159300000000009</v>
+        <v>7.83385</v>
       </c>
       <c r="J37">
-        <v>2.2001650971900002</v>
+        <v>9.6452557435299999E-2</v>
       </c>
       <c r="K37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="C38">
-        <v>76.91</v>
+        <v>78.5</v>
       </c>
       <c r="D38">
-        <v>2.3010000000000002</v>
+        <v>3.5030000000000001</v>
       </c>
       <c r="E38">
-        <v>0.69</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="F38">
-        <v>3240</v>
+        <v>5351</v>
       </c>
       <c r="G38">
-        <v>2189696</v>
+        <v>3330855</v>
       </c>
       <c r="H38">
-        <v>723</v>
+        <v>824</v>
       </c>
       <c r="I38">
-        <v>17.224900000000002</v>
+        <v>14.9473</v>
       </c>
       <c r="J38">
-        <v>1.23721317817</v>
+        <v>0.43545520851800001</v>
       </c>
       <c r="K38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>166</v>
-      </c>
-      <c r="B39" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39">
-        <v>79.23</v>
-      </c>
-      <c r="D39">
-        <v>1.702</v>
-      </c>
-      <c r="E39">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="F39">
-        <v>5323</v>
-      </c>
-      <c r="G39">
-        <v>2236126</v>
-      </c>
-      <c r="H39">
-        <v>498</v>
-      </c>
-      <c r="I39">
-        <v>4.9612499999999997</v>
-      </c>
-      <c r="J39">
-        <v>22.363607848699999</v>
-      </c>
-      <c r="K39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>150</v>
-      </c>
-      <c r="B40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C40">
+      <c r="C39" s="1">
         <v>91.15</v>
       </c>
-      <c r="D40">
+      <c r="D39" s="1">
         <v>0.8</v>
       </c>
-      <c r="E40">
+      <c r="E39" s="1">
         <v>0.65100000000000002</v>
       </c>
-      <c r="F40">
+      <c r="F39" s="1">
         <v>16850</v>
       </c>
-      <c r="G40">
+      <c r="G39" s="1">
         <v>2603423</v>
       </c>
-      <c r="H40">
+      <c r="H39" s="1">
         <v>216</v>
       </c>
-      <c r="I40">
+      <c r="I39" s="1">
         <v>25.537099999999999</v>
       </c>
-      <c r="J40">
+      <c r="J39" s="1">
         <v>0.18138352428999999</v>
       </c>
-      <c r="K40" t="s">
-        <v>95</v>
+      <c r="K39" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="1">
+        <v>90.29</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="F40" s="1">
+        <v>6411</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2721633</v>
+      </c>
+      <c r="H40" s="1">
+        <v>511</v>
+      </c>
+      <c r="I40" s="1">
+        <v>25.999300000000002</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0.204788098157</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="C41">
-        <v>77.81</v>
+        <v>74.92</v>
       </c>
       <c r="D41">
-        <v>3.23</v>
+        <v>1.615</v>
       </c>
       <c r="E41">
-        <v>0.71199999999999997</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="F41">
-        <v>3975</v>
+        <v>4719</v>
       </c>
       <c r="G41">
-        <v>2541424</v>
+        <v>2069396</v>
       </c>
       <c r="H41">
-        <v>794</v>
+        <v>480</v>
       </c>
       <c r="I41">
-        <v>21.505700000000001</v>
+        <v>6.5011400000000004</v>
       </c>
       <c r="J41">
-        <v>0.15969886688400001</v>
+        <v>9.6169606250399997E-2</v>
       </c>
       <c r="K41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C42">
-        <v>86.13</v>
+        <v>75.099999999999994</v>
       </c>
       <c r="D42">
-        <v>1.4</v>
+        <v>1.5329999999999999</v>
       </c>
       <c r="E42">
-        <v>0.67500000000000004</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="F42">
-        <v>7135</v>
+        <v>3129</v>
       </c>
       <c r="G42">
-        <v>2514956</v>
+        <v>1918756</v>
       </c>
       <c r="H42">
-        <v>453</v>
+        <v>665</v>
       </c>
       <c r="I42">
-        <v>10.4039</v>
+        <v>15.9353</v>
       </c>
       <c r="J42">
-        <v>0.24911757512499999</v>
+        <v>2.44123282253</v>
       </c>
       <c r="K42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -2471,1571 +2471,1571 @@
         <v>158</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="C43">
-        <v>84.64</v>
+        <v>82.18</v>
       </c>
       <c r="D43">
-        <v>3.8460000000000001</v>
+        <v>2.5529999999999999</v>
       </c>
       <c r="E43">
-        <v>0.70699999999999996</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="F43">
-        <v>9296</v>
+        <v>3574</v>
       </c>
       <c r="G43">
-        <v>2830978</v>
+        <v>2099664</v>
       </c>
       <c r="H43">
-        <v>394</v>
+        <v>658</v>
       </c>
       <c r="I43">
-        <v>7.6874599999999997</v>
+        <v>5.4398900000000001</v>
       </c>
       <c r="J43">
-        <v>1.04586346117</v>
+        <v>0.85196636327499997</v>
       </c>
       <c r="K43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="C44">
-        <v>97.05</v>
+        <v>72.47</v>
       </c>
       <c r="D44">
-        <v>0.81599999999999995</v>
+        <v>1.8</v>
       </c>
       <c r="E44">
-        <v>0.64300000000000002</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="F44">
-        <v>36692</v>
+        <v>3389</v>
       </c>
       <c r="G44">
-        <v>1787608</v>
+        <v>2173558</v>
       </c>
       <c r="H44">
-        <v>56</v>
+        <v>739</v>
       </c>
       <c r="I44">
-        <v>7.83385</v>
+        <v>56.4711</v>
       </c>
       <c r="J44">
-        <v>9.6452557435299999E-2</v>
+        <v>3.2386193518900002</v>
       </c>
       <c r="K44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="C45">
-        <v>98.01</v>
+        <v>72.989999999999995</v>
       </c>
       <c r="D45">
-        <v>1.702</v>
+        <v>1.2330000000000001</v>
       </c>
       <c r="E45">
-        <v>0.67600000000000005</v>
+        <v>0.66300000000000003</v>
       </c>
       <c r="F45">
-        <v>13193</v>
+        <v>5746</v>
       </c>
       <c r="G45">
-        <v>2907746</v>
+        <v>1892619</v>
       </c>
       <c r="H45">
-        <v>341</v>
+        <v>390</v>
       </c>
       <c r="I45">
-        <v>17.460899999999999</v>
+        <v>7.2593699999999997</v>
       </c>
       <c r="J45">
-        <v>4.4213335589999998</v>
+        <v>8.2451564577200003</v>
       </c>
       <c r="K45" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>174</v>
-      </c>
-      <c r="B46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46">
-        <v>75.099999999999994</v>
-      </c>
-      <c r="D46">
-        <v>1.5329999999999999</v>
-      </c>
-      <c r="E46">
-        <v>0.65800000000000003</v>
-      </c>
-      <c r="F46">
-        <v>3129</v>
-      </c>
-      <c r="G46">
-        <v>1918756</v>
-      </c>
-      <c r="H46">
-        <v>665</v>
-      </c>
-      <c r="I46">
-        <v>15.9353</v>
-      </c>
-      <c r="J46">
-        <v>2.44123282253</v>
-      </c>
-      <c r="K46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>147</v>
-      </c>
-      <c r="B47" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47">
-        <v>94.25</v>
-      </c>
-      <c r="D47">
-        <v>1.8660000000000001</v>
-      </c>
-      <c r="E47">
-        <v>0.70099999999999996</v>
-      </c>
-      <c r="F47">
-        <v>11609</v>
-      </c>
-      <c r="G47">
-        <v>3121721</v>
-      </c>
-      <c r="H47">
-        <v>374</v>
-      </c>
-      <c r="I47">
-        <v>22.2608</v>
-      </c>
-      <c r="J47">
-        <v>0.29722337135499999</v>
-      </c>
-      <c r="K47" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="1">
+        <v>94.84</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2.8149999999999999</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="F46" s="1">
+        <v>12192</v>
+      </c>
+      <c r="G46" s="1">
+        <v>3181126</v>
+      </c>
+      <c r="H46" s="1">
+        <v>354</v>
+      </c>
+      <c r="I46" s="1">
+        <v>9.5159300000000009</v>
+      </c>
+      <c r="J46" s="1">
+        <v>2.2001650971900002</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="1">
+        <v>74.23</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="F47" s="1">
+        <v>4858</v>
+      </c>
+      <c r="G47" s="1">
+        <v>2284265</v>
+      </c>
+      <c r="H47" s="1">
+        <v>602</v>
+      </c>
+      <c r="I47" s="1">
+        <v>9.5233399999999993</v>
+      </c>
+      <c r="J47" s="1">
+        <v>2.7439343193600001</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C48">
-        <v>78.22</v>
+        <v>78.790000000000006</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E48">
-        <v>0.68</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="F48">
-        <v>10518</v>
+        <v>3724</v>
       </c>
       <c r="G48">
-        <v>2572786</v>
+        <v>1469027</v>
       </c>
       <c r="H48">
-        <v>306</v>
+        <v>471</v>
       </c>
       <c r="I48">
-        <v>8.3396699999999999</v>
+        <v>13.3886</v>
       </c>
       <c r="J48">
-        <v>0.27717046590099997</v>
+        <v>2.84170697306</v>
       </c>
       <c r="K48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C49">
-        <v>90.29</v>
+        <v>73.94</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>2.0209999999999999</v>
       </c>
       <c r="E49">
-        <v>0.64500000000000002</v>
+        <v>0.67</v>
       </c>
       <c r="F49">
-        <v>6411</v>
+        <v>2547</v>
       </c>
       <c r="G49">
-        <v>2721633</v>
+        <v>1954103</v>
       </c>
       <c r="H49">
-        <v>511</v>
+        <v>787</v>
       </c>
       <c r="I49">
-        <v>25.999300000000002</v>
+        <v>221.91200000000001</v>
       </c>
       <c r="J49">
-        <v>0.204788098157</v>
+        <v>0.16151653510200001</v>
       </c>
       <c r="K49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="C50">
-        <v>74.92</v>
+        <v>72.180000000000007</v>
       </c>
       <c r="D50">
-        <v>1.615</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="E50">
-        <v>0.65200000000000002</v>
+        <v>0.66800000000000004</v>
       </c>
       <c r="F50">
-        <v>4719</v>
+        <v>8025</v>
       </c>
       <c r="G50">
-        <v>2069396</v>
+        <v>1841689</v>
       </c>
       <c r="H50">
-        <v>480</v>
+        <v>310</v>
       </c>
       <c r="I50">
-        <v>6.5011400000000004</v>
+        <v>5.4245700000000001</v>
       </c>
       <c r="J50">
-        <v>9.6169606250399997E-2</v>
+        <v>1.82360146632</v>
       </c>
       <c r="K50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C51">
-        <v>78.790000000000006</v>
+        <v>86.13</v>
       </c>
       <c r="D51">
-        <v>2.2000000000000002</v>
+        <v>1.4</v>
       </c>
       <c r="E51">
-        <v>0.67300000000000004</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="F51">
-        <v>3724</v>
+        <v>7135</v>
       </c>
       <c r="G51">
-        <v>1469027</v>
+        <v>2514956</v>
       </c>
       <c r="H51">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="I51">
-        <v>13.3886</v>
+        <v>10.4039</v>
       </c>
       <c r="J51">
-        <v>2.84170697306</v>
+        <v>0.24911757512499999</v>
       </c>
       <c r="K51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C52">
-        <v>86</v>
+        <v>74.03</v>
       </c>
       <c r="D52">
-        <v>3.6</v>
+        <v>1.2</v>
       </c>
       <c r="E52">
-        <v>0.69699999999999995</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="F52">
-        <v>7676</v>
+        <v>3137</v>
       </c>
       <c r="G52">
-        <v>2857481</v>
+        <v>2161520</v>
       </c>
       <c r="H52">
-        <v>467</v>
+        <v>755</v>
       </c>
       <c r="I52">
-        <v>7.3360000000000003</v>
+        <v>14.885199999999999</v>
       </c>
       <c r="J52">
-        <v>0.44963377502399998</v>
+        <v>1.9849744756100001</v>
       </c>
       <c r="K52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C53">
-        <v>73.94</v>
+        <v>98.01</v>
       </c>
       <c r="D53">
-        <v>2.0209999999999999</v>
+        <v>1.702</v>
       </c>
       <c r="E53">
-        <v>0.67</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="F53">
-        <v>2547</v>
+        <v>13193</v>
       </c>
       <c r="G53">
-        <v>1954103</v>
+        <v>2907746</v>
       </c>
       <c r="H53">
-        <v>787</v>
+        <v>341</v>
       </c>
       <c r="I53">
-        <v>221.91200000000001</v>
+        <v>17.460899999999999</v>
       </c>
       <c r="J53">
-        <v>0.16151653510200001</v>
+        <v>4.4213335589999998</v>
       </c>
       <c r="K53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C54">
-        <v>78.5</v>
+        <v>87.64</v>
       </c>
       <c r="D54">
-        <v>3.5030000000000001</v>
+        <v>2.133</v>
       </c>
       <c r="E54">
-        <v>0.65200000000000002</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="F54">
-        <v>5351</v>
+        <v>6167</v>
       </c>
       <c r="G54">
-        <v>3330855</v>
+        <v>2435471</v>
       </c>
       <c r="H54">
-        <v>824</v>
+        <v>441</v>
       </c>
       <c r="I54">
-        <v>14.9473</v>
+        <v>19.047599999999999</v>
       </c>
       <c r="J54">
-        <v>0.43545520851800001</v>
+        <v>11.062201458200001</v>
       </c>
       <c r="K54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C55">
-        <v>93.99</v>
+        <v>92.22</v>
       </c>
       <c r="D55">
-        <v>1.3149999999999999</v>
+        <v>2.056</v>
       </c>
       <c r="E55">
-        <v>0.61799999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="F55">
-        <v>9051</v>
+        <v>13407</v>
       </c>
       <c r="G55">
-        <v>2064438</v>
+        <v>2459580</v>
       </c>
       <c r="H55">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="I55">
-        <v>7.6235299999999997</v>
+        <v>29.417100000000001</v>
       </c>
       <c r="J55">
-        <v>0.17205142108599999</v>
+        <v>0.70663253125900005</v>
       </c>
       <c r="K55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="C56">
-        <v>82.87</v>
+        <v>81.87</v>
       </c>
       <c r="D56">
-        <v>2.7650000000000001</v>
+        <v>5.46</v>
       </c>
       <c r="E56">
-        <v>0.69699999999999995</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="F56">
-        <v>8057</v>
+        <v>4231</v>
       </c>
       <c r="G56">
-        <v>2446296</v>
+        <v>2422757</v>
       </c>
       <c r="H56">
-        <v>380</v>
+        <v>626</v>
       </c>
       <c r="I56">
-        <v>14.4673</v>
+        <v>34.419699999999999</v>
       </c>
       <c r="J56">
-        <v>0.72865067535799999</v>
+        <v>23.307644699899999</v>
       </c>
       <c r="K56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C57">
-        <v>89.84</v>
+        <v>78.22</v>
       </c>
       <c r="D57">
-        <v>1.47</v>
+        <v>5</v>
       </c>
       <c r="E57">
-        <v>0.59499999999999997</v>
+        <v>0.68</v>
       </c>
       <c r="F57">
-        <v>4846</v>
+        <v>10518</v>
       </c>
       <c r="G57">
-        <v>1906484</v>
+        <v>2572786</v>
       </c>
       <c r="H57">
-        <v>449</v>
+        <v>306</v>
       </c>
       <c r="I57">
-        <v>4.26478</v>
+        <v>8.3396699999999999</v>
       </c>
       <c r="J57">
-        <v>27.5250529333</v>
+        <v>0.27717046590099997</v>
       </c>
       <c r="K57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="C58">
-        <v>74.03</v>
+        <v>82.9</v>
       </c>
       <c r="D58">
-        <v>1.2</v>
+        <v>3.2970000000000002</v>
       </c>
       <c r="E58">
-        <v>0.68200000000000005</v>
+        <v>0.69</v>
       </c>
       <c r="F58">
-        <v>3137</v>
+        <v>4364</v>
       </c>
       <c r="G58">
-        <v>2161520</v>
+        <v>3093298</v>
       </c>
       <c r="H58">
-        <v>755</v>
+        <v>922</v>
       </c>
       <c r="I58">
-        <v>14.885199999999999</v>
+        <v>119.285</v>
       </c>
       <c r="J58">
-        <v>1.9849744756100001</v>
+        <v>3.13323336337</v>
       </c>
       <c r="K58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="C59">
-        <v>92.22</v>
+        <v>76.91</v>
       </c>
       <c r="D59">
-        <v>2.056</v>
+        <v>2.3010000000000002</v>
       </c>
       <c r="E59">
-        <v>0.68</v>
+        <v>0.69</v>
       </c>
       <c r="F59">
-        <v>13407</v>
+        <v>3240</v>
       </c>
       <c r="G59">
-        <v>2459580</v>
+        <v>2189696</v>
       </c>
       <c r="H59">
-        <v>273</v>
+        <v>723</v>
       </c>
       <c r="I59">
-        <v>29.417100000000001</v>
+        <v>17.224900000000002</v>
       </c>
       <c r="J59">
-        <v>0.70663253125900005</v>
+        <v>1.23721317817</v>
       </c>
       <c r="K59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="C60">
-        <v>87.64</v>
+        <v>75.150000000000006</v>
       </c>
       <c r="D60">
-        <v>2.133</v>
+        <v>2.2149999999999999</v>
       </c>
       <c r="E60">
-        <v>0.67600000000000005</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="F60">
-        <v>6167</v>
+        <v>2789</v>
       </c>
       <c r="G60">
-        <v>2435471</v>
+        <v>2616278</v>
       </c>
       <c r="H60">
-        <v>441</v>
+        <v>1008</v>
       </c>
       <c r="I60">
-        <v>19.047599999999999</v>
+        <v>49.792499999999997</v>
       </c>
       <c r="J60">
-        <v>11.062201458200001</v>
+        <v>0.52071066669099997</v>
       </c>
       <c r="K60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="B61" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="C61">
-        <v>81.040000000000006</v>
+        <v>89.63</v>
       </c>
       <c r="D61">
-        <v>3.133</v>
+        <v>2.3559999999999999</v>
       </c>
       <c r="E61">
-        <v>0.61299999999999999</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="F61">
-        <v>5061</v>
+        <v>12405</v>
       </c>
       <c r="G61">
-        <v>2694110</v>
+        <v>2703765</v>
       </c>
       <c r="H61">
-        <v>614</v>
+        <v>277</v>
       </c>
       <c r="I61">
-        <v>4.9092599999999997</v>
+        <v>8.4095300000000002</v>
       </c>
       <c r="J61">
-        <v>1.5635214425899999</v>
+        <v>1.6983139973200001</v>
       </c>
       <c r="K61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C62">
-        <v>82.18</v>
+        <v>82.87</v>
       </c>
       <c r="D62">
-        <v>2.5529999999999999</v>
+        <v>2.7650000000000001</v>
       </c>
       <c r="E62">
-        <v>0.66200000000000003</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="F62">
-        <v>3574</v>
+        <v>8057</v>
       </c>
       <c r="G62">
-        <v>2099664</v>
+        <v>2446296</v>
       </c>
       <c r="H62">
-        <v>658</v>
+        <v>380</v>
       </c>
       <c r="I62">
-        <v>5.4398900000000001</v>
+        <v>14.4673</v>
       </c>
       <c r="J62">
-        <v>0.85196636327499997</v>
+        <v>0.72865067535799999</v>
       </c>
       <c r="K62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C63">
-        <v>75.41</v>
+        <v>94.25</v>
       </c>
       <c r="D63">
-        <v>1.6459999999999999</v>
+        <v>1.8660000000000001</v>
       </c>
       <c r="E63">
         <v>0.70099999999999996</v>
       </c>
       <c r="F63">
-        <v>3002</v>
+        <v>11609</v>
       </c>
       <c r="G63">
-        <v>2346340</v>
+        <v>3121721</v>
       </c>
       <c r="H63">
-        <v>870</v>
+        <v>374</v>
       </c>
       <c r="I63">
-        <v>4.9122199999999996</v>
+        <v>22.2608</v>
       </c>
       <c r="J63">
-        <v>0.51766097284500001</v>
+        <v>0.29722337135499999</v>
       </c>
       <c r="K63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C64">
-        <v>70.58</v>
+        <v>75.41</v>
       </c>
       <c r="D64">
-        <v>4.8949999999999996</v>
+        <v>1.6459999999999999</v>
       </c>
       <c r="E64">
-        <v>0.70499999999999996</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="F64">
-        <v>3418</v>
+        <v>3002</v>
       </c>
       <c r="G64">
-        <v>2602320</v>
+        <v>2346340</v>
       </c>
       <c r="H64">
-        <v>861</v>
+        <v>870</v>
       </c>
       <c r="I64">
-        <v>5.3931100000000001</v>
+        <v>4.9122199999999996</v>
       </c>
       <c r="J64">
-        <v>0.89675532664199997</v>
+        <v>0.51766097284500001</v>
       </c>
       <c r="K64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="C65">
-        <v>74.23</v>
+        <v>87.75</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>1.762</v>
       </c>
       <c r="E65">
-        <v>0.67100000000000004</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="F65">
-        <v>4858</v>
+        <v>4711</v>
       </c>
       <c r="G65">
-        <v>2284265</v>
+        <v>2778251</v>
       </c>
       <c r="H65">
-        <v>602</v>
+        <v>636</v>
       </c>
       <c r="I65">
-        <v>9.5233399999999993</v>
+        <v>58.559199999999997</v>
       </c>
       <c r="J65">
-        <v>2.7439343193600001</v>
+        <v>0.66381948452299999</v>
       </c>
       <c r="K65" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>184</v>
-      </c>
-      <c r="B66" t="s">
-        <v>21</v>
-      </c>
-      <c r="C66">
-        <v>82.27</v>
-      </c>
-      <c r="D66">
-        <v>6.242</v>
-      </c>
-      <c r="E66">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="F66">
-        <v>4295</v>
-      </c>
-      <c r="G66">
-        <v>2400063</v>
-      </c>
-      <c r="H66">
-        <v>683</v>
-      </c>
-      <c r="I66">
-        <v>11.838800000000001</v>
-      </c>
-      <c r="J66">
-        <v>1.49179649714</v>
-      </c>
-      <c r="K66" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>183</v>
-      </c>
-      <c r="B67" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67">
-        <v>91.5</v>
-      </c>
-      <c r="D67">
-        <v>2.2719999999999998</v>
-      </c>
-      <c r="E67">
-        <v>0.65</v>
-      </c>
-      <c r="F67">
-        <v>7992</v>
-      </c>
-      <c r="G67">
-        <v>3721583</v>
-      </c>
-      <c r="H67">
-        <v>575</v>
-      </c>
-      <c r="I67">
-        <v>10.059900000000001</v>
-      </c>
-      <c r="J67">
-        <v>0.17827510887100001</v>
-      </c>
-      <c r="K67" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" s="1">
+        <v>81.7</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1.6659999999999999</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="F66" s="1">
+        <v>4157</v>
+      </c>
+      <c r="G66" s="1">
+        <v>2602580</v>
+      </c>
+      <c r="H66" s="1">
+        <v>689</v>
+      </c>
+      <c r="I66" s="1">
+        <v>7.2685000000000004</v>
+      </c>
+      <c r="J66" s="1">
+        <v>3.9312230735</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="1">
+        <v>86</v>
+      </c>
+      <c r="D67" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="F67" s="1">
+        <v>7676</v>
+      </c>
+      <c r="G67" s="1">
+        <v>2857481</v>
+      </c>
+      <c r="H67" s="1">
+        <v>467</v>
+      </c>
+      <c r="I67" s="1">
+        <v>7.3360000000000003</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0.44963377502399998</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C68">
-        <v>94.48</v>
+        <v>82.72</v>
       </c>
       <c r="D68">
-        <v>1.6739999999999999</v>
+        <v>4.415</v>
       </c>
       <c r="E68">
-        <v>0.69199999999999995</v>
+        <v>0.7</v>
       </c>
       <c r="F68">
-        <v>15045</v>
+        <v>6886</v>
       </c>
       <c r="G68">
-        <v>3252985</v>
+        <v>2162581</v>
       </c>
       <c r="H68">
-        <v>256</v>
+        <v>391</v>
       </c>
       <c r="I68">
-        <v>11.582800000000001</v>
+        <v>7.6546000000000003</v>
       </c>
       <c r="J68">
-        <v>1.92787913317</v>
+        <v>8.4782114963099993</v>
       </c>
       <c r="K68" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="B69" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="C69">
-        <v>75.48</v>
+        <v>86.96</v>
       </c>
       <c r="D69">
-        <v>0.90600000000000003</v>
+        <v>1.276</v>
       </c>
       <c r="E69">
-        <v>0.64200000000000002</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="F69">
-        <v>6027</v>
+        <v>4885</v>
       </c>
       <c r="G69">
-        <v>2636077</v>
+        <v>2115032</v>
       </c>
       <c r="H69">
-        <v>591</v>
+        <v>508</v>
       </c>
       <c r="I69">
-        <v>38.975099999999998</v>
+        <v>21.4267</v>
       </c>
       <c r="J69">
-        <v>5.5425214485900001E-3</v>
+        <v>0.85589581425299999</v>
       </c>
       <c r="K69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="C70">
-        <v>76.83</v>
+        <v>77.81</v>
       </c>
       <c r="D70">
-        <v>2.8039999999999998</v>
+        <v>3.23</v>
       </c>
       <c r="E70">
-        <v>0.71599999999999997</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="F70">
-        <v>3265</v>
+        <v>3975</v>
       </c>
       <c r="G70">
-        <v>2349948</v>
+        <v>2541424</v>
       </c>
       <c r="H70">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="I70">
-        <v>4.8772500000000001</v>
+        <v>21.505700000000001</v>
       </c>
       <c r="J70">
-        <v>2.67007662371</v>
+        <v>0.15969886688400001</v>
       </c>
       <c r="K70" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B71" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="C71">
-        <v>93.89</v>
+        <v>70.58</v>
       </c>
       <c r="D71">
-        <v>1.806</v>
+        <v>4.8949999999999996</v>
       </c>
       <c r="E71">
-        <v>0.68899999999999995</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="F71">
-        <v>11289</v>
+        <v>3418</v>
       </c>
       <c r="G71">
-        <v>2641672</v>
+        <v>2602320</v>
       </c>
       <c r="H71">
-        <v>327</v>
+        <v>861</v>
       </c>
       <c r="I71">
-        <v>9.1699199999999994</v>
+        <v>5.3931100000000001</v>
       </c>
       <c r="J71">
-        <v>4.6625713445399999</v>
+        <v>0.89675532664199997</v>
       </c>
       <c r="K71" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="B72" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C72">
-        <v>78.67</v>
+        <v>84.64</v>
       </c>
       <c r="D72">
-        <v>2.2810000000000001</v>
+        <v>3.8460000000000001</v>
       </c>
       <c r="E72">
-        <v>0.69299999999999995</v>
+        <v>0.70699999999999996</v>
       </c>
       <c r="F72">
-        <v>5589</v>
+        <v>9296</v>
       </c>
       <c r="G72">
-        <v>1966988</v>
+        <v>2830978</v>
       </c>
       <c r="H72">
-        <v>417</v>
+        <v>394</v>
       </c>
       <c r="I72">
-        <v>6.1789399999999999</v>
+        <v>7.6874599999999997</v>
       </c>
       <c r="J72">
-        <v>12.2381380991</v>
+        <v>1.04586346117</v>
       </c>
       <c r="K72" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B73" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C73">
-        <v>78.78</v>
+        <v>75.48</v>
       </c>
       <c r="D73">
-        <v>0.98199999999999998</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="E73">
-        <v>0.66700000000000004</v>
+        <v>0.64200000000000002</v>
       </c>
       <c r="F73">
-        <v>4286</v>
+        <v>6027</v>
       </c>
       <c r="G73">
-        <v>2172163</v>
+        <v>2636077</v>
       </c>
       <c r="H73">
-        <v>575</v>
+        <v>591</v>
       </c>
       <c r="I73">
-        <v>18.258500000000002</v>
+        <v>38.975099999999998</v>
       </c>
       <c r="J73">
-        <v>0.45491817023100001</v>
+        <v>5.5425214485900001E-3</v>
       </c>
       <c r="K73" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B74" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C74">
-        <v>94.6</v>
+        <v>91.5</v>
       </c>
       <c r="D74">
-        <v>1.8149999999999999</v>
+        <v>2.2719999999999998</v>
       </c>
       <c r="E74">
-        <v>0.64100000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="F74">
-        <v>11350</v>
+        <v>7992</v>
       </c>
       <c r="G74">
-        <v>3203868</v>
+        <v>3721583</v>
       </c>
       <c r="H74">
-        <v>355</v>
+        <v>575</v>
       </c>
       <c r="I74">
-        <v>9.3968100000000003</v>
+        <v>10.059900000000001</v>
       </c>
       <c r="J74">
-        <v>0.37106593092000001</v>
+        <v>0.17827510887100001</v>
       </c>
       <c r="K74" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C75">
-        <v>91.66</v>
+        <v>94.48</v>
       </c>
       <c r="D75">
-        <v>1.4530000000000001</v>
+        <v>1.6739999999999999</v>
       </c>
       <c r="E75">
-        <v>0.623</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="F75">
-        <v>14954</v>
+        <v>15045</v>
       </c>
       <c r="G75">
-        <v>3279077</v>
+        <v>3252985</v>
       </c>
       <c r="H75">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="I75">
-        <v>31.325700000000001</v>
+        <v>11.582800000000001</v>
       </c>
       <c r="J75">
-        <v>0.95599606681600002</v>
+        <v>1.92787913317</v>
       </c>
       <c r="K75" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C76">
-        <v>92.55</v>
+        <v>82.27</v>
       </c>
       <c r="D76">
-        <v>0.28199999999999997</v>
+        <v>6.242</v>
       </c>
       <c r="E76">
-        <v>0.63800000000000001</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="F76">
-        <v>8431</v>
+        <v>4295</v>
       </c>
       <c r="G76">
-        <v>3054377</v>
+        <v>2400063</v>
       </c>
       <c r="H76">
-        <v>447</v>
+        <v>683</v>
       </c>
       <c r="I76">
-        <v>6.9749400000000001</v>
+        <v>11.838800000000001</v>
       </c>
       <c r="J76">
-        <v>1.0578109834</v>
+        <v>1.49179649714</v>
       </c>
       <c r="K76" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B77" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C77">
-        <v>87.54</v>
+        <v>76.83</v>
       </c>
       <c r="D77">
-        <v>0.63400000000000001</v>
+        <v>2.8039999999999998</v>
       </c>
       <c r="E77">
-        <v>0.65800000000000003</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="F77">
-        <v>8878</v>
+        <v>3265</v>
       </c>
       <c r="G77">
-        <v>2437932</v>
+        <v>2349948</v>
       </c>
       <c r="H77">
-        <v>331</v>
+        <v>803</v>
       </c>
       <c r="I77">
-        <v>6.8994099999999996</v>
+        <v>4.8772500000000001</v>
       </c>
       <c r="J77">
-        <v>0.94897605457599998</v>
+        <v>2.67007662371</v>
       </c>
       <c r="K77" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C78">
-        <v>89.67</v>
+        <v>78.78</v>
       </c>
       <c r="D78">
-        <v>0.84699999999999998</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="E78">
-        <v>0.68</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="F78">
-        <v>4699</v>
+        <v>4286</v>
       </c>
       <c r="G78">
-        <v>2744797</v>
+        <v>2172163</v>
       </c>
       <c r="H78">
-        <v>603</v>
+        <v>575</v>
       </c>
       <c r="I78">
-        <v>40.635300000000001</v>
+        <v>18.258500000000002</v>
       </c>
       <c r="J78">
-        <v>0.56731724296399999</v>
+        <v>0.45491817023100001</v>
       </c>
       <c r="K78" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B79" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C79">
-        <v>82.92</v>
+        <v>78.67</v>
       </c>
       <c r="D79">
-        <v>0.56399999999999995</v>
+        <v>2.2810000000000001</v>
       </c>
       <c r="E79">
-        <v>0.68100000000000005</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="F79">
-        <v>3181</v>
+        <v>5589</v>
       </c>
       <c r="G79">
-        <v>2429326</v>
+        <v>1966988</v>
       </c>
       <c r="H79">
-        <v>764</v>
+        <v>417</v>
       </c>
       <c r="I79">
-        <v>38.553100000000001</v>
+        <v>6.1789399999999999</v>
       </c>
       <c r="J79">
-        <v>0.33092269493199999</v>
+        <v>12.2381380991</v>
       </c>
       <c r="K79" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B80" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C80">
-        <v>82.86</v>
+        <v>93.89</v>
       </c>
       <c r="D80">
-        <v>2.3639999999999999</v>
+        <v>1.806</v>
       </c>
       <c r="E80">
-        <v>0.61599999999999999</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="F80">
-        <v>5154</v>
+        <v>11289</v>
       </c>
       <c r="G80">
-        <v>3453679</v>
+        <v>2641672</v>
       </c>
       <c r="H80">
-        <v>778</v>
+        <v>327</v>
       </c>
       <c r="I80">
-        <v>4.7466699999999999</v>
+        <v>9.1699199999999994</v>
       </c>
       <c r="J80">
-        <v>2.64590920875</v>
+        <v>4.6625713445399999</v>
       </c>
       <c r="K80" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B81" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="C81">
-        <v>91.25</v>
+        <v>96.22</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1.333</v>
       </c>
       <c r="E81">
-        <v>0.64400000000000002</v>
+        <v>0.48299999999999998</v>
       </c>
       <c r="F81">
-        <v>8200</v>
+        <v>8198</v>
       </c>
       <c r="G81">
-        <v>2655338</v>
+        <v>3548370</v>
       </c>
       <c r="H81">
-        <v>419</v>
+        <v>599</v>
       </c>
       <c r="I81">
-        <v>5.77658</v>
+        <v>228.62100000000001</v>
       </c>
       <c r="J81">
-        <v>0.93849831142700002</v>
+        <v>0.429773399582</v>
       </c>
       <c r="K81" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B82" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C82">
-        <v>78.83</v>
+        <v>70.83</v>
       </c>
       <c r="D82">
-        <v>2.41</v>
+        <v>2.222</v>
       </c>
       <c r="E82">
-        <v>0.65800000000000003</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="F82">
-        <v>4365</v>
+        <v>3151</v>
       </c>
       <c r="G82">
-        <v>4202192</v>
+        <v>1667980</v>
       </c>
       <c r="H82">
-        <v>1030</v>
+        <v>534</v>
       </c>
       <c r="I82">
-        <v>4.6524599999999996</v>
+        <v>4.3306899999999997</v>
       </c>
       <c r="J82">
-        <v>0.10902753425099999</v>
+        <v>90.221264396600006</v>
       </c>
       <c r="K82" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>199</v>
+        <v>117</v>
       </c>
       <c r="B83" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C83">
-        <v>80.97</v>
+        <v>89.4</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1.869</v>
       </c>
       <c r="E83">
-        <v>0.45800000000000002</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="F83">
-        <v>5268</v>
+        <v>268131</v>
       </c>
       <c r="G83">
-        <v>616685</v>
+        <v>1037184</v>
       </c>
       <c r="H83">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="I83">
-        <v>7.5327400000000004</v>
+        <v>9.8953600000000002</v>
       </c>
       <c r="J83">
-        <v>4.4299352804899996</v>
+        <v>0.108350626666</v>
       </c>
       <c r="K83" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>201</v>
+        <v>119</v>
       </c>
       <c r="B84" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="C84">
-        <v>80.08</v>
+        <v>84.03</v>
       </c>
       <c r="D84">
-        <v>2.23</v>
+        <v>0</v>
       </c>
       <c r="E84">
-        <v>0.68799999999999994</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="F84">
-        <v>3687</v>
+        <v>13350</v>
       </c>
       <c r="G84">
-        <v>2200091</v>
+        <v>887108</v>
       </c>
       <c r="H84">
-        <v>568</v>
+        <v>85</v>
       </c>
       <c r="I84">
-        <v>22.8489</v>
+        <v>7.7114099999999999</v>
       </c>
       <c r="J84">
-        <v>0.94885614727099998</v>
+        <v>0.175100948422</v>
       </c>
       <c r="K84" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>200</v>
+        <v>118</v>
       </c>
       <c r="B85" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C85">
-        <v>81.03</v>
+        <v>87.14</v>
       </c>
       <c r="D85">
-        <v>1.724</v>
+        <v>0</v>
       </c>
       <c r="E85">
-        <v>0.502</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="F85">
-        <v>4473</v>
+        <v>43621</v>
       </c>
       <c r="G85">
-        <v>785653</v>
+        <v>1097787</v>
       </c>
       <c r="H85">
-        <v>226</v>
+        <v>35</v>
       </c>
       <c r="I85">
-        <v>6.4623999999999997</v>
+        <v>23.054200000000002</v>
       </c>
       <c r="J85">
-        <v>1.04182866076</v>
+        <v>0.15690615322699999</v>
       </c>
       <c r="K85" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C86">
-        <v>95.48</v>
+        <v>94.6</v>
       </c>
       <c r="D86">
-        <v>1.2070000000000001</v>
+        <v>1.8149999999999999</v>
       </c>
       <c r="E86">
-        <v>0.63700000000000001</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="F86">
-        <v>8367</v>
+        <v>11350</v>
       </c>
       <c r="G86">
-        <v>2396020</v>
+        <v>3203868</v>
       </c>
       <c r="H86">
-        <v>333</v>
+        <v>355</v>
       </c>
       <c r="I86">
-        <v>7.76295</v>
+        <v>9.3968100000000003</v>
       </c>
       <c r="J86">
-        <v>18.302453766599999</v>
+        <v>0.37106593092000001</v>
       </c>
       <c r="K86" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B87" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C87">
-        <v>81.540000000000006</v>
+        <v>91.66</v>
       </c>
       <c r="D87">
-        <v>1.6</v>
+        <v>1.4530000000000001</v>
       </c>
       <c r="E87">
-        <v>0.69699999999999995</v>
+        <v>0.623</v>
       </c>
       <c r="F87">
-        <v>4218</v>
+        <v>14954</v>
       </c>
       <c r="G87">
-        <v>2612197</v>
+        <v>3279077</v>
       </c>
       <c r="H87">
-        <v>725</v>
+        <v>286</v>
       </c>
       <c r="I87">
-        <v>5.6522800000000002</v>
+        <v>31.325700000000001</v>
       </c>
       <c r="J87">
-        <v>1.47342059872</v>
+        <v>0.95599606681600002</v>
       </c>
       <c r="K87" t="s">
         <v>101</v>
@@ -4043,34 +4043,34 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B88" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C88">
-        <v>85.75</v>
+        <v>82.86</v>
       </c>
       <c r="D88">
-        <v>0.8</v>
+        <v>2.3639999999999999</v>
       </c>
       <c r="E88">
-        <v>0.70599999999999996</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="F88">
-        <v>4801</v>
+        <v>5154</v>
       </c>
       <c r="G88">
-        <v>2415797</v>
+        <v>3453679</v>
       </c>
       <c r="H88">
-        <v>633</v>
+        <v>778</v>
       </c>
       <c r="I88">
-        <v>7.2144700000000004</v>
+        <v>4.7466699999999999</v>
       </c>
       <c r="J88">
-        <v>13.5394742311</v>
+        <v>2.64590920875</v>
       </c>
       <c r="K88" t="s">
         <v>101</v>
@@ -4078,34 +4078,34 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="B89" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C89">
-        <v>93.84</v>
+        <v>92.55</v>
       </c>
       <c r="D89">
-        <v>2.1360000000000001</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="E89">
-        <v>0.73</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="F89">
-        <v>11979</v>
+        <v>8431</v>
       </c>
       <c r="G89">
-        <v>2413993</v>
+        <v>3054377</v>
       </c>
       <c r="H89">
-        <v>200</v>
+        <v>447</v>
       </c>
       <c r="I89">
-        <v>18.581099999999999</v>
+        <v>6.9749400000000001</v>
       </c>
       <c r="J89">
-        <v>3.7820669748000002</v>
+        <v>1.0578109834</v>
       </c>
       <c r="K89" t="s">
         <v>101</v>
@@ -4113,182 +4113,112 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B90" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C90">
-        <v>97.77</v>
+        <v>87.54</v>
       </c>
       <c r="D90">
-        <v>0.222</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="E90">
-        <v>0.439</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="F90">
-        <v>18977</v>
+        <v>8878</v>
       </c>
       <c r="G90">
-        <v>3489855</v>
+        <v>2437932</v>
       </c>
       <c r="H90">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="I90">
-        <v>8.2834400000000006</v>
+        <v>6.8994099999999996</v>
       </c>
       <c r="J90">
-        <v>595.33637534000002</v>
+        <v>0.94897605457599998</v>
       </c>
       <c r="K90" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B91" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="C91">
-        <v>96.22</v>
+        <v>82.92</v>
       </c>
       <c r="D91">
-        <v>1.333</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="E91">
-        <v>0.48299999999999998</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="F91">
-        <v>8198</v>
+        <v>3181</v>
       </c>
       <c r="G91">
-        <v>3548370</v>
+        <v>2429326</v>
       </c>
       <c r="H91">
-        <v>599</v>
+        <v>764</v>
       </c>
       <c r="I91">
-        <v>228.62100000000001</v>
+        <v>38.553100000000001</v>
       </c>
       <c r="J91">
-        <v>0.429773399582</v>
+        <v>0.33092269493199999</v>
       </c>
       <c r="K91" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="B92" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="C92">
-        <v>70.83</v>
+        <v>89.67</v>
       </c>
       <c r="D92">
-        <v>2.222</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="E92">
-        <v>0.64700000000000002</v>
+        <v>0.68</v>
       </c>
       <c r="F92">
-        <v>3151</v>
+        <v>4699</v>
       </c>
       <c r="G92">
-        <v>1667980</v>
+        <v>2744797</v>
       </c>
       <c r="H92">
-        <v>534</v>
+        <v>603</v>
       </c>
       <c r="I92">
-        <v>4.3306899999999997</v>
+        <v>40.635300000000001</v>
       </c>
       <c r="J92">
-        <v>90.221264396600006</v>
+        <v>0.56731724296399999</v>
       </c>
       <c r="K92" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>209</v>
-      </c>
-      <c r="B93" t="s">
-        <v>92</v>
-      </c>
-      <c r="C93" t="s">
-        <v>97</v>
-      </c>
-      <c r="D93" t="s">
-        <v>97</v>
-      </c>
-      <c r="E93">
-        <v>0.55600000000000005</v>
-      </c>
-      <c r="F93">
-        <v>9621</v>
-      </c>
-      <c r="G93">
-        <v>9945709</v>
-      </c>
-      <c r="H93">
-        <v>901</v>
-      </c>
-      <c r="I93">
-        <v>23.713000000000001</v>
-      </c>
-      <c r="J93">
-        <v>1.4101678718699999</v>
-      </c>
-      <c r="K93" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>212</v>
-      </c>
-      <c r="B94" t="s">
-        <v>107</v>
-      </c>
-      <c r="C94" t="s">
-        <v>97</v>
-      </c>
-      <c r="D94" t="s">
-        <v>97</v>
-      </c>
-      <c r="E94">
-        <v>0.39500000000000002</v>
-      </c>
-      <c r="F94">
-        <v>36290</v>
-      </c>
-      <c r="G94">
-        <v>52519</v>
-      </c>
-      <c r="H94">
-        <v>29</v>
-      </c>
-      <c r="I94">
-        <v>179.339</v>
-      </c>
-      <c r="J94">
-        <v>1.4101678718699999</v>
-      </c>
-      <c r="K94" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K94">
-    <sortCondition ref="K2:K94"/>
+  <sortState ref="A2:K92">
+    <sortCondition ref="A2:A92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>